<commit_message>
Fixed comments and final code (debug leds  are commented)
</commit_message>
<xml_diff>
--- a/Design/Beta/bom/TX.xlsx
+++ b/Design/Beta/bom/TX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shantanusd/Documents/GitHub/Project-Flow/Design/Beta/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACE0F6C-1F75-084B-8B07-B0B52491EB5A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B6F848-A443-904A-A42A-AB42506D8DA7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XXX BOM-Edit" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0000000000"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -656,28 +656,28 @@
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1488,7 +1488,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>

</xml_diff>